<commit_message>
Commit new Godzilla V1
</commit_message>
<xml_diff>
--- a/3. Godzilla-market/Расходы.xlsx
+++ b/3. Godzilla-market/Расходы.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\муз мыси\Kwork\3. Godzilla-market\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Работа\Kwork\myKwork\3. Godzilla-market\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15032D18-EF3D-4DC0-A314-F19D754A76D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3985E16C-84A4-4702-85EC-0116CFAC3942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26670" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,15 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -63,7 +72,7 @@
     <t>Elementor Pro</t>
   </si>
   <si>
-    <t>RgZzfLb@5U4y</t>
+    <t>RS?MWck0c3Os</t>
   </si>
 </sst>
 </file>
@@ -402,6 +411,9 @@
     <xf numFmtId="164" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -422,9 +434,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -727,18 +736,18 @@
   <sheetData>
     <row r="2" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="19"/>
+      <c r="E3" s="20"/>
       <c r="I3" s="3"/>
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C4" s="23"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="12" t="s">
         <v>1</v>
       </c>
@@ -749,7 +758,7 @@
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C5" s="23"/>
+      <c r="C5" s="24"/>
       <c r="D5" s="4" t="s">
         <v>2</v>
       </c>
@@ -758,7 +767,7 @@
       </c>
     </row>
     <row r="6" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C6" s="23"/>
+      <c r="C6" s="24"/>
       <c r="D6" s="6" t="s">
         <v>5</v>
       </c>
@@ -767,23 +776,23 @@
       </c>
     </row>
     <row r="7" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="23"/>
+      <c r="C7" s="24"/>
       <c r="D7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="18" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="23"/>
-      <c r="D8" s="20" t="s">
+      <c r="C8" s="24"/>
+      <c r="D8" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="21"/>
+      <c r="E8" s="22"/>
     </row>
     <row r="9" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C9" s="23"/>
+      <c r="C9" s="24"/>
       <c r="D9" s="11" t="s">
         <v>10</v>
       </c>
@@ -792,7 +801,7 @@
       </c>
     </row>
     <row r="10" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C10" s="23"/>
+      <c r="C10" s="24"/>
       <c r="D10" s="8" t="s">
         <v>11</v>
       </c>
@@ -801,22 +810,22 @@
       </c>
     </row>
     <row r="11" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C11" s="23"/>
+      <c r="C11" s="24"/>
       <c r="D11" s="8"/>
       <c r="E11" s="15"/>
     </row>
     <row r="12" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C12" s="23"/>
+      <c r="C12" s="24"/>
       <c r="D12" s="8"/>
       <c r="E12" s="15"/>
     </row>
     <row r="13" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C13" s="23"/>
+      <c r="C13" s="24"/>
       <c r="D13" s="8"/>
       <c r="E13" s="15"/>
     </row>
     <row r="14" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C14" s="23"/>
+      <c r="C14" s="24"/>
       <c r="D14" s="8"/>
       <c r="E14" s="15"/>
       <c r="P14" s="2"/>
@@ -824,7 +833,7 @@
       <c r="V14" s="2"/>
     </row>
     <row r="15" spans="3:22" x14ac:dyDescent="0.2">
-      <c r="C15" s="23"/>
+      <c r="C15" s="24"/>
       <c r="D15" s="8"/>
       <c r="E15" s="15"/>
       <c r="P15" s="2"/>
@@ -832,7 +841,7 @@
       <c r="V15" s="2"/>
     </row>
     <row r="16" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="24"/>
+      <c r="C16" s="25"/>
       <c r="D16" s="9"/>
       <c r="E16" s="16"/>
       <c r="P16" s="2"/>
@@ -852,7 +861,7 @@
   <hyperlinks>
     <hyperlink ref="E4" r:id="rId1" xr:uid="{6DA402B8-76A2-497D-A29E-518D31C30C1B}"/>
     <hyperlink ref="E5" r:id="rId2" xr:uid="{29DA5A94-4E63-4E99-A814-7C4480BAA11C}"/>
-    <hyperlink ref="E7" r:id="rId3" xr:uid="{40DE8952-C0D7-403A-A80C-E5213D823005}"/>
+    <hyperlink ref="E7" r:id="rId3" display="RgZzfLb@5U4y" xr:uid="{40DE8952-C0D7-403A-A80C-E5213D823005}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>